<commit_message>
refactored the code to make it neater
- all attributes are now camelCase
- missing information will no longer have a key
</commit_message>
<xml_diff>
--- a/telegram-bot/entities/mylibs/FormattedCarparkRates.xlsx
+++ b/telegram-bot/entities/mylibs/FormattedCarparkRates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\SNDGG-SMU-IS483\NGSI-LD-SG-Datamall\mylibs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\SNDGG-SMU-IS483\telegram-bot\entities\mylibs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316C5B09-9622-4DCB-9EEC-04A38B840574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE31777-985C-46DE-81FE-7AF17E30A6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>saturday</t>
   </si>
   <si>
-    <t>sunday_public_holiday</t>
-  </si>
-  <si>
     <t>Bedok Mall</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>06:59</t>
+  </si>
+  <si>
+    <t>sundayPublicHoliday</t>
   </si>
 </sst>
 </file>
@@ -621,8 +621,8 @@
   <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4">
         <v>4.5</v>
@@ -775,10 +775,10 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -874,7 +874,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8">
         <v>4.5</v>
@@ -903,10 +903,10 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -932,7 +932,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -964,7 +964,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -993,16 +993,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>1.5</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1089,25 +1089,25 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
       </c>
       <c r="E15">
         <v>2.2200000000000002</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15">
         <v>2.5</v>
@@ -1121,13 +1121,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1136,10 +1136,10 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16">
         <v>2.5</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -1162,7 +1162,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>2.2200000000000002</v>
@@ -1185,16 +1185,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>2.2200000000000002</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
@@ -1258,7 +1258,7 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20">
         <v>2.14</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -1313,16 +1313,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22">
         <v>2.14</v>
@@ -1345,16 +1345,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
-      </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1377,16 +1377,16 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
@@ -1418,7 +1418,7 @@
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1441,16 +1441,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1473,13 +1473,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
         <v>16</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -1514,7 +1514,7 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28">
         <v>4.5</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
@@ -1546,7 +1546,7 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E29">
         <v>4.5</v>
@@ -1569,16 +1569,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30">
         <v>4.5</v>
@@ -1601,16 +1601,16 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
         <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" t="s">
-        <v>31</v>
       </c>
       <c r="E31">
         <v>2.14</v>
@@ -1633,16 +1633,16 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
         <v>32</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
       </c>
       <c r="E32">
         <v>2.14</v>
@@ -1665,16 +1665,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33">
         <v>2.14</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
@@ -1706,7 +1706,7 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34">
         <v>2.14</v>
@@ -1729,16 +1729,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E35">
         <v>2.14</v>
@@ -1761,13 +1761,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
         <v>16</v>
@@ -1779,7 +1779,7 @@
         <v>16</v>
       </c>
       <c r="G36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H36">
         <v>3.75</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
@@ -1802,7 +1802,7 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E37">
         <v>2.14</v>
@@ -1811,7 +1811,7 @@
         <v>16</v>
       </c>
       <c r="G37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37">
         <v>3.75</v>
@@ -1825,16 +1825,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E38">
         <v>2.14</v>
@@ -1843,7 +1843,7 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H38">
         <v>3.75</v>
@@ -1857,16 +1857,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
         <v>24</v>
-      </c>
-      <c r="D39" t="s">
-        <v>25</v>
       </c>
       <c r="E39">
         <v>2.14</v>
@@ -1889,16 +1889,16 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E40">
         <v>3.53</v>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
@@ -1930,7 +1930,7 @@
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E41">
         <v>3.53</v>
@@ -1953,16 +1953,16 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E42">
         <v>3.53</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
         <v>11</v>
@@ -1994,7 +1994,7 @@
         <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43">
         <v>2.14</v>
@@ -2003,7 +2003,7 @@
         <v>16</v>
       </c>
       <c r="G43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H43">
         <v>2.14</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44" t="s">
         <v>18</v>
@@ -2026,7 +2026,7 @@
         <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44">
         <v>2.14</v>
@@ -2049,16 +2049,16 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E45">
         <v>2.14</v>
@@ -2081,13 +2081,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
         <v>16</v>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>11</v>
@@ -2122,7 +2122,7 @@
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47">
         <v>2.4</v>
@@ -2145,7 +2145,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
         <v>18</v>
@@ -2154,7 +2154,7 @@
         <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E48">
         <v>1.2</v>
@@ -2177,16 +2177,16 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C49" t="s">
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E49">
         <v>1.2</v>
@@ -2209,7 +2209,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
@@ -2224,7 +2224,7 @@
         <v>14</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G50" t="s">
         <v>16</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
         <v>18</v>
@@ -2256,7 +2256,7 @@
         <v>14</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G51" t="s">
         <v>16</v>
@@ -2273,10 +2273,10 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
         <v>14</v>
@@ -2288,7 +2288,7 @@
         <v>14</v>
       </c>
       <c r="F52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G52" t="s">
         <v>16</v>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
         <v>11</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
         <v>18</v>
@@ -2369,10 +2369,10 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -2401,16 +2401,16 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E56">
         <v>2.67</v>
@@ -2433,16 +2433,16 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E57">
         <v>3</v>
@@ -2465,7 +2465,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
@@ -2474,7 +2474,7 @@
         <v>12</v>
       </c>
       <c r="D58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E58">
         <v>2.56</v>
@@ -2497,16 +2497,16 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E59">
         <v>2.56</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
@@ -2538,7 +2538,7 @@
         <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E60">
         <v>1.07</v>
@@ -2547,7 +2547,7 @@
         <v>16</v>
       </c>
       <c r="G60" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H60">
         <v>2.14</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B61" t="s">
         <v>18</v>
@@ -2570,7 +2570,7 @@
         <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E61">
         <v>2.14</v>
@@ -2593,16 +2593,16 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
         <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E62">
         <v>2.14</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
@@ -2634,7 +2634,7 @@
         <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E63">
         <v>1.07</v>
@@ -2643,7 +2643,7 @@
         <v>16</v>
       </c>
       <c r="G63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H63">
         <v>2.14</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B64" t="s">
         <v>18</v>
@@ -2666,7 +2666,7 @@
         <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E64">
         <v>2.14</v>
@@ -2689,16 +2689,16 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E65">
         <v>2.14</v>
@@ -2721,16 +2721,16 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E66">
         <v>2.2000000000000002</v>
@@ -2753,16 +2753,16 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
       </c>
       <c r="C67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E67">
         <v>2.2000000000000002</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B68" t="s">
         <v>18</v>
@@ -2794,7 +2794,7 @@
         <v>12</v>
       </c>
       <c r="D68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E68">
         <v>2.4</v>
@@ -2817,16 +2817,16 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C69" t="s">
         <v>12</v>
       </c>
       <c r="D69" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E69">
         <v>2.4</v>
@@ -2849,13 +2849,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D70" t="s">
         <v>16</v>
@@ -2867,7 +2867,7 @@
         <v>16</v>
       </c>
       <c r="G70" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H70">
         <v>2.2000000000000002</v>
@@ -2881,7 +2881,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B71" t="s">
         <v>18</v>
@@ -2890,7 +2890,7 @@
         <v>12</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E71">
         <v>2.2000000000000002</v>
@@ -2913,16 +2913,16 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E72">
         <v>2.2000000000000002</v>
@@ -2945,7 +2945,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B73" t="s">
         <v>11</v>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B74" t="s">
         <v>18</v>
@@ -3009,10 +3009,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B75" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C75" t="s">
         <v>14</v>
@@ -3041,16 +3041,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" t="s">
         <v>47</v>
       </c>
-      <c r="B76" t="s">
-        <v>11</v>
-      </c>
-      <c r="C76" t="s">
-        <v>48</v>
-      </c>
       <c r="D76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E76">
         <v>1.28</v>
@@ -3073,16 +3073,16 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B77" t="s">
         <v>11</v>
       </c>
       <c r="C77" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" t="s">
         <v>49</v>
-      </c>
-      <c r="D77" t="s">
-        <v>50</v>
       </c>
       <c r="E77">
         <v>1.82</v>
@@ -3105,16 +3105,16 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D78" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E78">
         <v>1.82</v>
@@ -3137,16 +3137,16 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B79" t="s">
         <v>11</v>
       </c>
       <c r="C79" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" t="s">
         <v>51</v>
-      </c>
-      <c r="D79" t="s">
-        <v>52</v>
       </c>
       <c r="E79">
         <v>4.28</v>
@@ -3169,7 +3169,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B80" t="s">
         <v>18</v>
@@ -3178,7 +3178,7 @@
         <v>12</v>
       </c>
       <c r="D80" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E80">
         <v>2.57</v>
@@ -3201,16 +3201,16 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B81" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C81" t="s">
         <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E81">
         <v>2.57</v>
@@ -3233,13 +3233,13 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D82" t="s">
         <v>16</v>
@@ -3251,7 +3251,7 @@
         <v>16</v>
       </c>
       <c r="G82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H82">
         <v>4.5</v>
@@ -3265,7 +3265,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B83" t="s">
         <v>18</v>
@@ -3274,7 +3274,7 @@
         <v>12</v>
       </c>
       <c r="D83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E83">
         <v>4.5</v>
@@ -3297,16 +3297,16 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C84" t="s">
         <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E84">
         <v>4.5</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B85" t="s">
         <v>11</v>
@@ -3338,7 +3338,7 @@
         <v>12</v>
       </c>
       <c r="D85" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E85">
         <v>3</v>
@@ -3347,7 +3347,7 @@
         <v>16</v>
       </c>
       <c r="G85" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H85">
         <v>4.8</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B86" t="s">
         <v>18</v>
@@ -3370,7 +3370,7 @@
         <v>12</v>
       </c>
       <c r="D86" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E86">
         <v>4.8</v>
@@ -3393,16 +3393,16 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
         <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E87">
         <v>4.8</v>
@@ -3425,25 +3425,25 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B88" t="s">
         <v>11</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E88">
         <v>2</v>
       </c>
       <c r="F88" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H88">
         <v>2</v>
@@ -3457,7 +3457,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B89" t="s">
         <v>18</v>
@@ -3466,7 +3466,7 @@
         <v>12</v>
       </c>
       <c r="D89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E89">
         <v>2</v>
@@ -3489,16 +3489,16 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B90" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C90" t="s">
         <v>12</v>
       </c>
       <c r="D90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E90">
         <v>2</v>
@@ -3521,16 +3521,16 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>55</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91" t="s">
         <v>56</v>
       </c>
-      <c r="B91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>57</v>
-      </c>
-      <c r="D91" t="s">
-        <v>58</v>
       </c>
       <c r="E91">
         <v>2.58</v>
@@ -3539,7 +3539,7 @@
         <v>16</v>
       </c>
       <c r="G91" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H91">
         <v>3.48</v>
@@ -3553,7 +3553,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B92" t="s">
         <v>18</v>
@@ -3562,7 +3562,7 @@
         <v>12</v>
       </c>
       <c r="D92" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E92">
         <v>3.48</v>
@@ -3585,16 +3585,16 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>55</v>
+      </c>
+      <c r="B93" t="s">
+        <v>81</v>
+      </c>
+      <c r="C93" t="s">
         <v>56</v>
       </c>
-      <c r="B93" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>57</v>
-      </c>
-      <c r="D93" t="s">
-        <v>58</v>
       </c>
       <c r="E93">
         <v>3.48</v>
@@ -3603,7 +3603,7 @@
         <v>16</v>
       </c>
       <c r="G93" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H93">
         <v>3.48</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
@@ -3626,7 +3626,7 @@
         <v>12</v>
       </c>
       <c r="D94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E94">
         <v>1.07</v>
@@ -3635,7 +3635,7 @@
         <v>16</v>
       </c>
       <c r="G94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H94">
         <v>2.14</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B95" t="s">
         <v>18</v>
@@ -3658,7 +3658,7 @@
         <v>12</v>
       </c>
       <c r="D95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E95">
         <v>2.14</v>
@@ -3681,16 +3681,16 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C96" t="s">
         <v>12</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E96">
         <v>2.14</v>
@@ -3713,16 +3713,16 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B97" t="s">
         <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D97" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E97">
         <v>2.2000000000000002</v>
@@ -3731,7 +3731,7 @@
         <v>16</v>
       </c>
       <c r="G97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H97">
         <v>3</v>
@@ -3745,7 +3745,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B98" t="s">
         <v>18</v>
@@ -3754,7 +3754,7 @@
         <v>12</v>
       </c>
       <c r="D98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E98">
         <v>3</v>
@@ -3777,16 +3777,16 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B99" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C99" t="s">
         <v>12</v>
       </c>
       <c r="D99" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E99">
         <v>3</v>
@@ -3809,25 +3809,25 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B100" t="s">
         <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D100" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E100">
         <v>7</v>
       </c>
       <c r="F100" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G100" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H100">
         <v>6</v>
@@ -3841,25 +3841,25 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B101" t="s">
         <v>18</v>
       </c>
       <c r="C101" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D101" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E101">
         <v>8</v>
       </c>
       <c r="F101" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H101">
         <v>8</v>
@@ -3873,25 +3873,25 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B102" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C102" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E102">
         <v>8</v>
       </c>
       <c r="F102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G102" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H102">
         <v>8</v>
@@ -3905,25 +3905,25 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B103" t="s">
         <v>11</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D103" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E103">
         <v>3</v>
       </c>
       <c r="F103" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G103" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H103">
         <v>2</v>
@@ -3937,7 +3937,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B104" t="s">
         <v>18</v>
@@ -3946,7 +3946,7 @@
         <v>12</v>
       </c>
       <c r="D104" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E104">
         <v>5</v>
@@ -3969,16 +3969,16 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B105" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C105" t="s">
         <v>12</v>
       </c>
       <c r="D105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E105">
         <v>5</v>
@@ -4001,25 +4001,25 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B106" t="s">
         <v>11</v>
       </c>
       <c r="C106" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D106" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E106">
         <v>3</v>
       </c>
       <c r="F106" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G106" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H106">
         <v>2</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B107" t="s">
         <v>18</v>
@@ -4042,7 +4042,7 @@
         <v>12</v>
       </c>
       <c r="D107" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E107">
         <v>5</v>
@@ -4065,16 +4065,16 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B108" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C108" t="s">
         <v>12</v>
       </c>
       <c r="D108" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E108">
         <v>5</v>
@@ -4097,7 +4097,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B109" t="s">
         <v>11</v>
@@ -4115,7 +4115,7 @@
         <v>16</v>
       </c>
       <c r="G109" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H109">
         <v>2</v>
@@ -4129,7 +4129,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B110" t="s">
         <v>18</v>
@@ -4138,7 +4138,7 @@
         <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E110">
         <v>2</v>
@@ -4161,16 +4161,16 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B111" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C111" t="s">
         <v>12</v>
       </c>
       <c r="D111" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E111">
         <v>2</v>
@@ -4193,25 +4193,25 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B112" t="s">
         <v>11</v>
       </c>
       <c r="C112" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D112" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E112">
         <v>2.2000000000000002</v>
       </c>
       <c r="F112" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G112" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H112">
         <v>2.2000000000000002</v>
@@ -4225,7 +4225,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B113" t="s">
         <v>18</v>
@@ -4234,7 +4234,7 @@
         <v>12</v>
       </c>
       <c r="D113" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E113">
         <v>1.1000000000000001</v>
@@ -4257,16 +4257,16 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B114" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C114" t="s">
         <v>12</v>
       </c>
       <c r="D114" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E114">
         <v>1.1000000000000001</v>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B115" t="s">
         <v>11</v>
@@ -4298,7 +4298,7 @@
         <v>12</v>
       </c>
       <c r="D115" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E115">
         <v>1.07</v>
@@ -4307,7 +4307,7 @@
         <v>16</v>
       </c>
       <c r="G115" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H115">
         <v>2.14</v>
@@ -4321,7 +4321,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B116" t="s">
         <v>18</v>
@@ -4330,7 +4330,7 @@
         <v>12</v>
       </c>
       <c r="D116" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E116">
         <v>2.14</v>
@@ -4353,16 +4353,16 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B117" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
       </c>
       <c r="D117" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E117">
         <v>2.14</v>
@@ -4385,7 +4385,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B118" t="s">
         <v>11</v>
@@ -4403,7 +4403,7 @@
         <v>16</v>
       </c>
       <c r="G118" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H118">
         <v>6</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B119" t="s">
         <v>18</v>
@@ -4426,7 +4426,7 @@
         <v>12</v>
       </c>
       <c r="D119" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E119">
         <v>6</v>
@@ -4449,16 +4449,16 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B120" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C120" t="s">
         <v>12</v>
       </c>
       <c r="D120" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E120">
         <v>6</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B121" t="s">
         <v>11</v>
@@ -4490,7 +4490,7 @@
         <v>12</v>
       </c>
       <c r="D121" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E121">
         <v>1.07</v>
@@ -4499,7 +4499,7 @@
         <v>16</v>
       </c>
       <c r="G121" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H121">
         <v>2.14</v>
@@ -4513,7 +4513,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B122" t="s">
         <v>18</v>
@@ -4522,7 +4522,7 @@
         <v>12</v>
       </c>
       <c r="D122" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E122">
         <v>2.14</v>
@@ -4545,16 +4545,16 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B123" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C123" t="s">
         <v>12</v>
       </c>
       <c r="D123" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E123">
         <v>2.14</v>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B124" t="s">
         <v>11</v>
@@ -4595,7 +4595,7 @@
         <v>16</v>
       </c>
       <c r="G124" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H124">
         <v>2</v>
@@ -4609,7 +4609,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B125" t="s">
         <v>18</v>
@@ -4618,7 +4618,7 @@
         <v>12</v>
       </c>
       <c r="D125" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E125">
         <v>2</v>
@@ -4641,16 +4641,16 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B126" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C126" t="s">
         <v>12</v>
       </c>
       <c r="D126" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E126">
         <v>2</v>
@@ -4673,16 +4673,16 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B127" t="s">
         <v>11</v>
       </c>
       <c r="C127" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D127" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E127">
         <v>1.5</v>
@@ -4705,7 +4705,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B128" t="s">
         <v>18</v>
@@ -4714,7 +4714,7 @@
         <v>12</v>
       </c>
       <c r="D128" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E128">
         <v>1.5</v>
@@ -4737,16 +4737,16 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B129" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C129" t="s">
         <v>12</v>
       </c>
       <c r="D129" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E129">
         <v>1.5</v>
@@ -4769,13 +4769,13 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B130" t="s">
         <v>11</v>
       </c>
       <c r="C130" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D130" t="s">
         <v>16</v>
@@ -4787,7 +4787,7 @@
         <v>16</v>
       </c>
       <c r="G130" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H130">
         <v>3</v>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B131" t="s">
         <v>18</v>
@@ -4810,7 +4810,7 @@
         <v>12</v>
       </c>
       <c r="D131" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E131">
         <v>1.4</v>
@@ -4833,16 +4833,16 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B132" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C132" t="s">
         <v>12</v>
       </c>
       <c r="D132" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E132">
         <v>1.4</v>
@@ -4865,13 +4865,13 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B133" t="s">
         <v>11</v>
       </c>
       <c r="C133" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D133" t="s">
         <v>16</v>
@@ -4883,7 +4883,7 @@
         <v>16</v>
       </c>
       <c r="G133" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H133">
         <v>3</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B134" t="s">
         <v>18</v>
@@ -4906,7 +4906,7 @@
         <v>12</v>
       </c>
       <c r="D134" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E134">
         <v>1.4</v>
@@ -4929,16 +4929,16 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B135" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C135" t="s">
         <v>12</v>
       </c>
       <c r="D135" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E135">
         <v>1.4</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B136" t="s">
         <v>11</v>
@@ -4970,7 +4970,7 @@
         <v>12</v>
       </c>
       <c r="D136" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E136">
         <v>3</v>
@@ -4979,7 +4979,7 @@
         <v>16</v>
       </c>
       <c r="G136" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H136">
         <v>4.8</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B137" t="s">
         <v>18</v>
@@ -5002,7 +5002,7 @@
         <v>12</v>
       </c>
       <c r="D137" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E137">
         <v>4.8</v>
@@ -5025,16 +5025,16 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B138" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C138" t="s">
         <v>12</v>
       </c>
       <c r="D138" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E138">
         <v>4.8</v>
@@ -5057,13 +5057,13 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B139" t="s">
         <v>11</v>
       </c>
       <c r="C139" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D139" t="s">
         <v>16</v>
@@ -5075,7 +5075,7 @@
         <v>16</v>
       </c>
       <c r="G139" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H139">
         <v>4.5</v>
@@ -5089,7 +5089,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B140" t="s">
         <v>18</v>
@@ -5098,7 +5098,7 @@
         <v>12</v>
       </c>
       <c r="D140" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E140">
         <v>4.5</v>
@@ -5121,16 +5121,16 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B141" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C141" t="s">
         <v>12</v>
       </c>
       <c r="D141" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E141">
         <v>4.5</v>
@@ -5153,25 +5153,25 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B142" t="s">
         <v>11</v>
       </c>
       <c r="C142" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D142" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E142">
         <v>2.4</v>
       </c>
       <c r="F142" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G142" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H142">
         <v>3.5</v>
@@ -5185,7 +5185,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B143" t="s">
         <v>18</v>
@@ -5194,7 +5194,7 @@
         <v>12</v>
       </c>
       <c r="D143" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E143">
         <v>3.6</v>
@@ -5217,16 +5217,16 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B144" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="C144" t="s">
         <v>12</v>
       </c>
       <c r="D144" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E144">
         <v>3.6</v>

</xml_diff>